<commit_message>
data provider test and final tests
</commit_message>
<xml_diff>
--- a/Assignment2/src/test/java/page_object_model/resources/TestData.xlsx
+++ b/Assignment2/src/test/java/page_object_model/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\uni\yr 4\SEMESTER 1\IS4102 Advanced Software Quality Assurance\ASQA-assignment-2\Assignment2\src\test\java\page_object_model\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49FC709C-DB4C-4374-9364-4036DFA7D43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ACB392-DC22-4E5B-8235-CB85E2FD2A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8FCD4A05-98A6-4F63-965E-B5210E9E0C5A}"/>
   </bookViews>
@@ -56,20 +56,20 @@
     <t>Failure</t>
   </si>
   <si>
-    <t>correctPass</t>
-  </si>
-  <si>
-    <t>correctUsername</t>
-  </si>
-  <si>
     <t>Success</t>
+  </si>
+  <si>
+    <t>12345678m@</t>
+  </si>
+  <si>
+    <t>michellenikeetha@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,10 +80,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,13 +116,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,17 +465,18 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,51 +487,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>